<commit_message>
Update import curriculum class
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C712F240-56AB-4B76-A1CC-0D246EC06874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5770754-C655-418B-996A-929EAF074E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIÊU CHUẨN- phân công GV K28" sheetId="1" r:id="rId1"/>
@@ -5425,10 +5425,10 @@
     <t>CS2.C.03.09</t>
   </si>
   <si>
-    <t xml:space="preserve">Tên HP   </t>
-  </si>
-  <si>
-    <t>Ghi chú 1</t>
+    <t xml:space="preserve">Tên HP      </t>
+  </si>
+  <si>
+    <t>Ghi Chú 1</t>
   </si>
 </sst>
 </file>
@@ -6349,7 +6349,7 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>

</xml_diff>